<commit_message>
pre v3.2 e v3.3
</commit_message>
<xml_diff>
--- a/presentazione/tempi.xlsx
+++ b/presentazione/tempi.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="10950" windowHeight="6585"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="11">
   <si>
     <t>Tempi presentazione</t>
   </si>
@@ -230,12 +230,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -249,11 +243,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -552,7 +552,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -564,36 +564,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="3" spans="1:6">
       <c r="B3" s="1"/>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="13" t="s">
+      <c r="D4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="12" t="s">
         <v>6</v>
       </c>
     </row>
@@ -624,7 +624,7 @@
       <c r="D6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="13">
         <v>56</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -641,7 +641,7 @@
       <c r="D7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="13">
         <v>20</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -652,11 +652,15 @@
       <c r="B8" s="2">
         <v>4</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="4">
+        <v>22</v>
+      </c>
       <c r="D8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="16"/>
+      <c r="E8" s="13">
+        <v>35</v>
+      </c>
       <c r="F8" s="2" t="s">
         <v>10</v>
       </c>
@@ -665,34 +669,52 @@
       <c r="B9" s="2">
         <v>5</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="4">
+        <v>24</v>
+      </c>
       <c r="D9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="2"/>
+      <c r="E9" s="13">
+        <v>32</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
       <c r="B10" s="2">
         <v>6</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="4">
+        <v>21</v>
+      </c>
       <c r="D10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="2"/>
+      <c r="E10" s="13">
+        <v>16</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:6">
       <c r="B11" s="2">
         <v>7</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="4">
+        <v>19</v>
+      </c>
       <c r="D11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="2"/>
+      <c r="E11" s="13">
+        <v>19</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="B12" s="2">
@@ -702,8 +724,10 @@
       <c r="D12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="2"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:6">
       <c r="B13" s="2">
@@ -713,8 +737,10 @@
       <c r="D13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="2"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="B14" s="2">
@@ -724,7 +750,7 @@
       <c r="D14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="16"/>
+      <c r="E14" s="13"/>
       <c r="F14" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix pre v3.4 e 3.4_flat
</commit_message>
<xml_diff>
--- a/presentazione/tempi.xlsx
+++ b/presentazione/tempi.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="10950" windowHeight="6585"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="10035" windowHeight="6570"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="29">
   <si>
     <t>Tempi presentazione</t>
   </si>
@@ -61,6 +61,48 @@
   </si>
   <si>
     <t>03</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>00</t>
   </si>
 </sst>
 </file>
@@ -223,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -242,6 +284,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -250,25 +310,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -564,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -579,21 +620,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="3" spans="1:7">
       <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
     </row>
     <row r="4" spans="1:7">
       <c r="B4" s="3" t="s">
@@ -616,13 +657,13 @@
       <c r="B5" s="2">
         <v>1</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="8">
         <v>37</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="13">
+      <c r="D5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="10">
         <v>20</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -633,13 +674,13 @@
       <c r="B6" s="2">
         <v>2</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="13">
         <v>29</v>
       </c>
-      <c r="D6" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="16">
+      <c r="D6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="12">
         <v>56</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -650,13 +691,13 @@
       <c r="B7" s="2">
         <v>3</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="13">
         <v>22</v>
       </c>
-      <c r="D7" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="16">
+      <c r="D7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="12">
         <v>20</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -667,13 +708,13 @@
       <c r="B8" s="2">
         <v>4</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="13">
         <v>22</v>
       </c>
-      <c r="D8" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="16">
+      <c r="D8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="12">
         <v>35</v>
       </c>
       <c r="F8" s="2" t="s">
@@ -684,13 +725,13 @@
       <c r="B9" s="2">
         <v>5</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="13">
         <v>24</v>
       </c>
-      <c r="D9" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="16">
+      <c r="D9" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="12">
         <v>32</v>
       </c>
       <c r="F9" s="2" t="s">
@@ -701,13 +742,13 @@
       <c r="B10" s="2">
         <v>6</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="13">
         <v>21</v>
       </c>
-      <c r="D10" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="16">
+      <c r="D10" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="12">
         <v>16</v>
       </c>
       <c r="F10" s="2" t="s">
@@ -718,13 +759,13 @@
       <c r="B11" s="2">
         <v>7</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="13">
         <v>19</v>
       </c>
-      <c r="D11" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="16">
+      <c r="D11" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="12">
         <v>19</v>
       </c>
       <c r="F11" s="2" t="s">
@@ -735,13 +776,13 @@
       <c r="B12" s="2">
         <v>8</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="13">
         <v>15</v>
       </c>
-      <c r="D12" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="16">
+      <c r="D12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="12">
         <v>50</v>
       </c>
       <c r="F12" s="2" t="s">
@@ -755,13 +796,13 @@
       <c r="B13" s="2">
         <v>9</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="13">
         <v>18</v>
       </c>
-      <c r="D13" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="16" t="s">
+      <c r="D13" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="12" t="s">
         <v>14</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -775,12 +816,178 @@
       <c r="B14" s="2">
         <v>10</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="16"/>
+      <c r="C14" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>16</v>
+      </c>
       <c r="F14" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="B15" s="2">
+        <v>11</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" s="2">
+        <v>12</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="2">
+        <v>13</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="2">
+        <v>14</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="2">
+        <v>15</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="2">
+        <v>16</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="2">
+        <v>17</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" s="2">
+        <v>18</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" s="2">
+        <v>19</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="12"/>
+      <c r="F23" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24" s="2">
+        <v>20</v>
+      </c>
+      <c r="C24" s="13"/>
+      <c r="D24" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="12"/>
+      <c r="F24" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -791,6 +998,9 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="C14:C18 E13:E14 E15:E18" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>